<commit_message>
Cleanup obsolete files and cache directories
- Remove old CSV output files (ranked_top25_*.csv, screener_latest_*.csv, top_*_plan.csv)
- Remove experimental/advanced features that were incomplete or unused:
  - Indmoney broker integration (indmoney_gtt.py, indmoney_token_manager.py)
  - LLM news summarization (llm_news_summarizer.py)
  - Multi-agent RL (multi_agent_rl.py)
  - News sentiment analysis (news_sentiment.py)
  - RL agent (rl_agent.py)
  - Self-enhancement features (self_enhance.py, ultimate_self_enhance.py)
- Remove test files for experimental features (test_autonomous_enhancements.py, test_ultimate_enhancement.py, tests/test_gtt_reconciler.py)
- Clean up all __pycache__ directories (automatically regenerated)
- Repository is now cleaner with only active, functional code
</commit_message>
<xml_diff>
--- a/outputs/gtt/GTT_Delivery_Live_Final.xlsx
+++ b/outputs/gtt/GTT_Delivery_Live_Final.xlsx
@@ -42,7 +42,7 @@
       <sz val="14"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -53,6 +53,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00CCCCCC"/>
         <bgColor rgb="00CCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C8E6C9"/>
+        <bgColor rgb="00C8E6C9"/>
       </patternFill>
     </fill>
     <fill>
@@ -74,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -82,6 +88,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -447,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,7 +481,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Generated: 2025-12-25 23:40:37 IST</t>
+          <t>Generated: 2026-01-07 15:01:01 IST</t>
         </is>
       </c>
     </row>
@@ -498,7 +505,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Total Positions: 4</t>
+          <t>Total Positions: 10</t>
         </is>
       </c>
     </row>
@@ -510,7 +517,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Total Value: ₹192,167</t>
+          <t>Total Value: ₹3,790,656</t>
         </is>
       </c>
     </row>
@@ -522,14 +529,49 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Total Risk: ₹83</t>
+          <t>Total Risk: ₹33</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="E8" t="inlineStr">
         <is>
-          <t>Average Confidence: 0.1/5</t>
+          <t>Average Confidence: 0.2/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Entry Methodology:</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>N/A Strategy:</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>• Entry: Pullback to EMA20 with RSI/MACD confirmation</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>• Stop Loss: ATR-based below entry</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>• Target: 2:1 risk-reward ratio</t>
         </is>
       </c>
     </row>
@@ -544,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AN12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +629,11 @@
     <col width="15" customWidth="1" min="33" max="33"/>
     <col width="15" customWidth="1" min="34" max="34"/>
     <col width="15" customWidth="1" min="35" max="35"/>
+    <col width="15" customWidth="1" min="36" max="36"/>
+    <col width="15" customWidth="1" min="37" max="37"/>
+    <col width="15" customWidth="1" min="38" max="38"/>
+    <col width="15" customWidth="1" min="39" max="39"/>
+    <col width="15" customWidth="1" min="40" max="40"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -604,170 +651,195 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
+          <t>Strategy</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="D2" s="5" t="inlineStr">
         <is>
           <t>ENTRY_trigger_price</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="E2" s="5" t="inlineStr">
         <is>
           <t>TARGET_trigger_price</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="F2" s="5" t="inlineStr">
         <is>
           <t>STOPLOSS_trigger_price</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="G2" s="5" t="inlineStr">
         <is>
           <t>DecisionConfidence</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Confidence_Level</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="I2" s="5" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>Explanation</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="K2" s="5" t="inlineStr">
         <is>
           <t>GTT_Explanation</t>
         </is>
       </c>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
+        <is>
+          <t>AVWAP60</t>
+        </is>
+      </c>
+      <c r="M2" s="5" t="inlineStr">
+        <is>
+          <t>EMA20</t>
+        </is>
+      </c>
+      <c r="N2" s="5" t="inlineStr">
+        <is>
+          <t>EMA50</t>
+        </is>
+      </c>
+      <c r="O2" s="5" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="P2" s="5" t="inlineStr">
+        <is>
+          <t>Entry_Logic</t>
+        </is>
+      </c>
+      <c r="Q2" s="5" t="inlineStr">
+        <is>
+          <t>Stop_Logic</t>
+        </is>
+      </c>
+      <c r="R2" s="5" t="inlineStr">
+        <is>
+          <t>Target_Logic</t>
+        </is>
+      </c>
+      <c r="S2" s="5" t="inlineStr">
         <is>
           <t>RSI14_D</t>
         </is>
       </c>
-      <c r="L2" s="5" t="inlineStr">
+      <c r="T2" s="5" t="inlineStr">
         <is>
           <t>RSI_Above50_D</t>
         </is>
       </c>
-      <c r="M2" s="5" t="inlineStr">
+      <c r="U2" s="5" t="inlineStr">
         <is>
           <t>RSI_Overbought_D</t>
         </is>
       </c>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="V2" s="5" t="inlineStr">
         <is>
           <t>MACD_Line_D</t>
         </is>
       </c>
-      <c r="O2" s="5" t="inlineStr">
+      <c r="W2" s="5" t="inlineStr">
         <is>
           <t>MACD_Signal_D</t>
         </is>
       </c>
-      <c r="P2" s="5" t="inlineStr">
+      <c r="X2" s="5" t="inlineStr">
         <is>
           <t>MACD_Hist_D</t>
         </is>
       </c>
-      <c r="Q2" s="5" t="inlineStr">
+      <c r="Y2" s="5" t="inlineStr">
         <is>
           <t>MACD_CrossUp_D</t>
         </is>
       </c>
-      <c r="R2" s="5" t="inlineStr">
+      <c r="Z2" s="5" t="inlineStr">
         <is>
           <t>MACD_AboveZero_D</t>
         </is>
       </c>
-      <c r="S2" s="5" t="inlineStr">
+      <c r="AA2" s="5" t="inlineStr">
         <is>
           <t>RSI14_H4</t>
         </is>
       </c>
-      <c r="T2" s="5" t="inlineStr">
+      <c r="AB2" s="5" t="inlineStr">
         <is>
           <t>RSI_Above50_H4</t>
         </is>
       </c>
-      <c r="U2" s="5" t="inlineStr">
+      <c r="AC2" s="5" t="inlineStr">
         <is>
           <t>MACD_CrossUp_H4</t>
         </is>
       </c>
-      <c r="V2" s="5" t="inlineStr">
+      <c r="AD2" s="5" t="inlineStr">
         <is>
           <t>RSI_MACD_Confirmations_OK</t>
         </is>
       </c>
-      <c r="W2" s="5" t="inlineStr">
+      <c r="AE2" s="5" t="inlineStr">
         <is>
           <t>RSI_MACD_Notes</t>
         </is>
       </c>
-      <c r="X2" s="5" t="inlineStr">
+      <c r="AF2" s="5" t="inlineStr">
         <is>
           <t>Audit_Flag</t>
         </is>
       </c>
-      <c r="Y2" s="5" t="inlineStr">
+      <c r="AG2" s="5" t="inlineStr">
         <is>
           <t>Issues</t>
         </is>
       </c>
-      <c r="Z2" s="5" t="inlineStr">
+      <c r="AH2" s="5" t="inlineStr">
         <is>
           <t>Fix_Suggestion</t>
         </is>
       </c>
-      <c r="AA2" s="5" t="inlineStr">
+      <c r="AI2" s="5" t="inlineStr">
         <is>
           <t>Pivot_Source</t>
         </is>
       </c>
-      <c r="AB2" s="5" t="inlineStr">
-        <is>
-          <t>Entry_Logic</t>
-        </is>
-      </c>
-      <c r="AC2" s="5" t="inlineStr">
-        <is>
-          <t>Stop_Logic</t>
-        </is>
-      </c>
-      <c r="AD2" s="5" t="inlineStr">
-        <is>
-          <t>Target_Logic</t>
-        </is>
-      </c>
-      <c r="AE2" s="5" t="inlineStr">
+      <c r="AJ2" s="5" t="inlineStr">
         <is>
           <t>Latest_Close</t>
         </is>
       </c>
-      <c r="AF2" s="5" t="inlineStr">
+      <c r="AK2" s="5" t="inlineStr">
         <is>
           <t>Latest_LTP</t>
         </is>
       </c>
-      <c r="AG2" s="5" t="inlineStr">
+      <c r="AL2" s="5" t="inlineStr">
         <is>
           <t>Canonical_Entry</t>
         </is>
       </c>
-      <c r="AH2" s="5" t="inlineStr">
+      <c r="AM2" s="5" t="inlineStr">
         <is>
           <t>Canonical_Stop</t>
         </is>
       </c>
-      <c r="AI2" s="5" t="inlineStr">
+      <c r="AN2" s="5" t="inlineStr">
         <is>
           <t>Canonical_Target</t>
         </is>
@@ -776,306 +848,340 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RELIANCE</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>36</v>
+          <t>SETFNIFBK</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>1514.64</v>
+        <v>127</v>
       </c>
       <c r="D3" t="n">
-        <v>1569.63</v>
+        <v>604.83</v>
       </c>
       <c r="E3" t="n">
-        <v>1487.15</v>
+        <v>620.47</v>
       </c>
       <c r="F3" s="6" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="n">
+        <v>597</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
         <v>2</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=1514.64 (BELOW), Stop=1487.15 (ATR×1.5), Target=1569.63 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at </t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="n">
-        <v>60.04</v>
-      </c>
-      <c r="L3" t="b">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=604.83 (BELOW), Stop=597.00 (ATR×1.5), Target=620.47 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Don</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="n">
+        <v>594.72</v>
+      </c>
+      <c r="M3" t="n">
+        <v>604.83</v>
+      </c>
+      <c r="N3" t="n">
+        <v>598.9299999999999</v>
+      </c>
+      <c r="O3" t="n">
+        <v>606.15</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 604.83</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹598.93</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>50.86</v>
+      </c>
+      <c r="T3" t="b">
         <v>1</v>
       </c>
-      <c r="M3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>81.79259999999999</v>
-      </c>
-      <c r="O3" t="n">
-        <v>108.4743</v>
-      </c>
-      <c r="P3" t="n">
-        <v>-26.6817</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" t="b">
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>1.0462</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1.7719</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-0.7257</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="b">
         <v>1</v>
       </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="b">
-        <v>0</v>
-      </c>
-      <c r="U3" t="b">
-        <v>0</v>
-      </c>
-      <c r="V3" t="b">
-        <v>0</v>
-      </c>
-      <c r="W3" t="inlineStr">
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="inlineStr">
         <is>
           <t>RSI/MACD fail</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>FAIL</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>ENTRY deviates 2.8% from canonical (1558.20)</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>Use canonical ENTRY=1558.20 from Close; Ensure all prices are tick-rounded to NSE EQ standard (₹0.05)</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG3" t="n">
+        <v/>
+      </c>
+      <c r="AH3" t="n">
+        <v/>
+      </c>
+      <c r="AI3" t="inlineStr">
         <is>
           <t>Close</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>Entry at Close (1558.20)</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>Stop 1.5x ATR below entry (ATR=18.33)</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>Target 2.0R from entry (Risk=27.50)</t>
-        </is>
-      </c>
-      <c r="AE3" t="n">
-        <v>1558.2</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>1558.2</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>1558.2</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>1530.7</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>1613.2</v>
+      <c r="AJ3" t="n">
+        <v>606.15</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>606.15</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>606.15</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>598.35</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>621.75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>INFY</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>23</v>
+          <t>SBILIQETF</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>1609.02</v>
+        <v>257</v>
       </c>
       <c r="D4" t="n">
-        <v>1692.85</v>
+        <v>1018.48</v>
       </c>
       <c r="E4" t="n">
-        <v>1567.11</v>
+        <v>1026.25</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
+        <v>1014.59</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
         <v>2</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=1609.02 (BELOW), Stop=1567.11 (ATR×1.5), Target=1692.85 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at </t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="n">
-        <v>65.76000000000001</v>
-      </c>
-      <c r="L4" t="b">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=1018.48 (BELOW), Stop=1014.59 (ATR×1.5), Target=1026.25 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at </t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>1018</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1018.48</v>
+      </c>
+      <c r="N4" t="n">
+        <v>996.13</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1020.55</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 1018.48</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹996.13</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>100</v>
+      </c>
+      <c r="T4" t="b">
         <v>1</v>
       </c>
-      <c r="M4" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>34.1928</v>
-      </c>
-      <c r="O4" t="n">
-        <v>29.4087</v>
-      </c>
-      <c r="P4" t="n">
-        <v>4.784</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" t="b">
+      <c r="U4" t="b">
         <v>1</v>
       </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="b">
-        <v>0</v>
-      </c>
-      <c r="U4" t="b">
-        <v>0</v>
-      </c>
-      <c r="V4" t="b">
-        <v>0</v>
-      </c>
-      <c r="W4" t="inlineStr">
+      <c r="V4" t="n">
+        <v>2.0668</v>
+      </c>
+      <c r="W4" t="n">
+        <v>2.3563</v>
+      </c>
+      <c r="X4" t="n">
+        <v>-0.2895</v>
+      </c>
+      <c r="Y4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="inlineStr">
         <is>
           <t>RSI/MACD fail</t>
         </is>
       </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>FAIL</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>ENTRY deviates 3.3% from canonical (1663.40)</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>Use canonical ENTRY=1663.40 from Close; Ensure all prices are tick-rounded to NSE EQ standard (₹0.05)</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG4" t="n">
+        <v/>
+      </c>
+      <c r="AH4" t="n">
+        <v/>
+      </c>
+      <c r="AI4" t="inlineStr">
         <is>
           <t>Close</t>
         </is>
       </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>Entry at Close (1663.40)</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>Stop 1.5x ATR below entry (ATR=27.94)</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>Target 2.0R from entry (Risk=41.90)</t>
-        </is>
-      </c>
-      <c r="AE4" t="n">
-        <v>1663.4</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>1663.4</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>1663.4</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>1621.5</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>1747.2</v>
+      <c r="AJ4" t="n">
+        <v>1020.55</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>1020.55</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>1020.55</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>1016.65</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>1028.35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NIFTYBEES</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>176</v>
+          <t>MOM30IETF</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
       </c>
       <c r="C5" t="n">
-        <v>333.6</v>
+        <v>1498</v>
       </c>
       <c r="D5" t="n">
-        <v>344.96</v>
+        <v>31.92</v>
       </c>
       <c r="E5" t="n">
-        <v>327.92</v>
+        <v>33.25</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
         <v>2</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=333.60 (BELOW), Stop=327.92 (ATR×1.5), Target=344.96 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Don</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="n">
-        <v>53.45</v>
-      </c>
-      <c r="L5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" t="b">
-        <v>0</v>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=31.92 (BELOW), Stop=31.25 (ATR×1.5), Target=33.25 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Donchi</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>31.94</v>
+      </c>
+      <c r="M5" t="n">
+        <v>31.92</v>
       </c>
       <c r="N5" t="n">
-        <v>-83.96729999999999</v>
+        <v>31.94</v>
       </c>
       <c r="O5" t="n">
-        <v>-116.5205</v>
-      </c>
-      <c r="P5" t="n">
-        <v>32.5531</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R5" t="b">
-        <v>0</v>
+        <v>31.77</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 31.92</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹31.94</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>49.44</v>
       </c>
       <c r="T5" t="b">
         <v>0</v>
@@ -1083,186 +1189,1020 @@
       <c r="U5" t="b">
         <v>0</v>
       </c>
-      <c r="V5" t="b">
-        <v>0</v>
-      </c>
-      <c r="W5" t="inlineStr">
+      <c r="V5" t="n">
+        <v>-0.1093</v>
+      </c>
+      <c r="W5" t="n">
+        <v>-0.0984</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-0.0109</v>
+      </c>
+      <c r="Y5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="inlineStr">
         <is>
           <t>RSI/MACD fail</t>
         </is>
       </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>FAIL</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>ENTRY deviates 12.9% from canonical (295.50)</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>Use canonical ENTRY=295.50 from Close; Ensure all prices are tick-rounded to NSE EQ standard (₹0.05)</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG5" t="n">
+        <v/>
+      </c>
+      <c r="AH5" t="n">
+        <v/>
+      </c>
+      <c r="AI5" t="inlineStr">
         <is>
           <t>Close</t>
         </is>
       </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>Entry at Close (295.50)</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>Stop 1.5x ATR below entry (ATR=3.79)</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>Target 2.0R from entry (Risk=5.70)</t>
-        </is>
-      </c>
-      <c r="AE5" t="n">
-        <v>295.5</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>295.5</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>295.5</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>289.8</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>306.9</v>
+      <c r="AJ5" t="n">
+        <v>31.77</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>31.77</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>31.75</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>33.05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SETFNIF50</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>133</v>
+          <t>FINIETF</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
       </c>
       <c r="C6" t="n">
-        <v>315.18</v>
+        <v>1148</v>
       </c>
       <c r="D6" t="n">
-        <v>330.13</v>
+        <v>32.34</v>
       </c>
       <c r="E6" t="n">
-        <v>307.71</v>
+        <v>34.08</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="n">
+        <v>31.47</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
         <v>2</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=315.18 (BELOW), Stop=307.71 (ATR×1.5), Target=330.13 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Don</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>52.6</v>
-      </c>
-      <c r="L6" t="b">
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=32.34 (BELOW), Stop=31.47 (ATR×1.5), Target=34.08 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Donchi</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>32.15</v>
+      </c>
+      <c r="M6" t="n">
+        <v>32.34</v>
+      </c>
+      <c r="N6" t="n">
+        <v>32.05</v>
+      </c>
+      <c r="O6" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 32.34</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹32.05</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>51.41</v>
+      </c>
+      <c r="T6" t="b">
         <v>1</v>
       </c>
-      <c r="M6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>-76.7617</v>
-      </c>
-      <c r="O6" t="n">
-        <v>-106.2182</v>
-      </c>
-      <c r="P6" t="n">
-        <v>29.4565</v>
-      </c>
-      <c r="Q6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="b">
-        <v>0</v>
-      </c>
       <c r="U6" t="b">
         <v>0</v>
       </c>
-      <c r="V6" t="b">
-        <v>0</v>
-      </c>
-      <c r="W6" t="inlineStr">
+      <c r="V6" t="n">
+        <v>0.0594</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.0579</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="Y6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="inlineStr">
         <is>
           <t>RSI/MACD fail</t>
         </is>
       </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>FAIL</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>ENTRY deviates 12.8% from canonical (279.30)</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>Use canonical ENTRY=279.30 from Close; Ensure all prices are tick-rounded to NSE EQ standard (₹0.05)</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG6" t="n">
+        <v/>
+      </c>
+      <c r="AH6" t="n">
+        <v/>
+      </c>
+      <c r="AI6" t="inlineStr">
         <is>
           <t>Close</t>
         </is>
       </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>Entry at Close (279.30)</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>Stop 1.5x ATR below entry (ATR=4.98)</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>Target 2.0R from entry (Risk=7.50)</t>
-        </is>
-      </c>
-      <c r="AE6" t="n">
-        <v>279.3</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>279.3</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>279.3</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>271.8</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>294.3</v>
+      <c r="AJ6" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>32.27</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>32.25</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>33.95</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>NIFTYETF</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>251</v>
+      </c>
+      <c r="D7" t="n">
+        <v>280.53</v>
+      </c>
+      <c r="E7" t="n">
+        <v>288.48</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>276.55</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=280.53 (BELOW), Stop=276.55 (ATR×1.5), Target=288.48 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Don</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>279.29</v>
+      </c>
+      <c r="M7" t="n">
+        <v>280.53</v>
+      </c>
+      <c r="N7" t="n">
+        <v>278.79</v>
+      </c>
+      <c r="O7" t="n">
+        <v>280.2</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 280.53</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹278.79</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>53.77</v>
+      </c>
+      <c r="T7" t="b">
+        <v>1</v>
+      </c>
+      <c r="U7" t="b">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.3774</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.4932</v>
+      </c>
+      <c r="X7" t="n">
+        <v>-0.1159</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>RSI/MACD fail</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG7" t="n">
+        <v/>
+      </c>
+      <c r="AH7" t="n">
+        <v/>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="AJ7" t="n">
+        <v>280.2</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>280.2</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>280.2</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>276.2</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>288.2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ITETF</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>792</v>
+      </c>
+      <c r="D8" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="E8" t="n">
+        <v>42.54</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>38.75</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=40.01 (BELOW), Stop=38.75 (ATR×1.5), Target=42.54 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Donchi</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>38.6</v>
+      </c>
+      <c r="M8" t="n">
+        <v>40.01</v>
+      </c>
+      <c r="N8" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>39.77</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 40.01</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹39.1</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>48.62</v>
+      </c>
+      <c r="T8" t="b">
+        <v>0</v>
+      </c>
+      <c r="U8" t="b">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.5602</v>
+      </c>
+      <c r="X8" t="n">
+        <v>-0.1183</v>
+      </c>
+      <c r="Y8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>RSI/MACD fail</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG8" t="n">
+        <v/>
+      </c>
+      <c r="AH8" t="n">
+        <v/>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="AJ8" t="n">
+        <v>39.77</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>39.77</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>39.75</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>42.25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>BSLSENETFG</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>341</v>
+      </c>
+      <c r="D9" t="n">
+        <v>85.05</v>
+      </c>
+      <c r="E9" t="n">
+        <v>90.91</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>82.12</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=85.05 (BELOW), Stop=82.12 (ATR×1.5), Target=90.91 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Donchi</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>84.39</v>
+      </c>
+      <c r="M9" t="n">
+        <v>85.05</v>
+      </c>
+      <c r="N9" t="n">
+        <v>84.48</v>
+      </c>
+      <c r="O9" t="n">
+        <v>85.05</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 85.05</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹84.48</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
+      </c>
+      <c r="S9" t="n">
+        <v>52.74</v>
+      </c>
+      <c r="T9" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" t="b">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.1213</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.1742</v>
+      </c>
+      <c r="X9" t="n">
+        <v>-0.0529</v>
+      </c>
+      <c r="Y9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>RSI/MACD fail</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG9" t="n">
+        <v/>
+      </c>
+      <c r="AH9" t="n">
+        <v/>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="AJ9" t="n">
+        <v>85.05</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>85.05</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>85.05000000000001</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>82.10000000000001</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>90.95</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>LIQUIDBETF</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>2953</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1060.94</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1061.62</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>1060.6</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=1060.94 (BELOW), Stop=1060.60 (ATR×1.5), Target=1061.62 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at </t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>1056.48</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1060.94</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1057.85</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1062.95</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 1060.94</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹1057.85</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
+        <v>100</v>
+      </c>
+      <c r="T10" t="b">
+        <v>1</v>
+      </c>
+      <c r="U10" t="b">
+        <v>1</v>
+      </c>
+      <c r="V10" t="n">
+        <v>1.438</v>
+      </c>
+      <c r="W10" t="n">
+        <v>1.4149</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.0231</v>
+      </c>
+      <c r="Y10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>RSI/MACD fail</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG10" t="n">
+        <v/>
+      </c>
+      <c r="AH10" t="n">
+        <v/>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="AJ10" t="n">
+        <v>1062.95</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>1062.95</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>1062.95</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>1062.6</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>1063.65</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BANKBEES</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>122</v>
+      </c>
+      <c r="D11" t="n">
+        <v>609.67</v>
+      </c>
+      <c r="E11" t="n">
+        <v>626.03</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v>601.48</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=609.67 (BELOW), Stop=601.48 (ATR×1.5), Target=626.03 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Don</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="n">
+        <v>600.88</v>
+      </c>
+      <c r="M11" t="n">
+        <v>609.67</v>
+      </c>
+      <c r="N11" t="n">
+        <v>603.84</v>
+      </c>
+      <c r="O11" t="n">
+        <v>611.5599999999999</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 609.67</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹603.84</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
+      </c>
+      <c r="S11" t="n">
+        <v>52.49</v>
+      </c>
+      <c r="T11" t="b">
+        <v>1</v>
+      </c>
+      <c r="U11" t="b">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.9986</v>
+      </c>
+      <c r="W11" t="n">
+        <v>1.691</v>
+      </c>
+      <c r="X11" t="n">
+        <v>-0.6925</v>
+      </c>
+      <c r="Y11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>RSI/MACD fail</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG11" t="n">
+        <v/>
+      </c>
+      <c r="AH11" t="n">
+        <v/>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="AJ11" t="n">
+        <v>611.5599999999999</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>611.5599999999999</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>611.5500000000001</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>603.35</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>627.95</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>PSUBNKBEES</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CompositeScore</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>310</v>
+      </c>
+      <c r="D12" t="n">
+        <v>92.62</v>
+      </c>
+      <c r="E12" t="n">
+        <v>99.06</v>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v>89.40000000000001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.2195972082891347</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Selected via CompositeScore fallback (no active signals): ranked by score using RS_ROC20, RVOL20, Trend_OK, breakout flags. Entry=92.62 (BELOW), Stop=89.40 (ATR×1.5), Target=99.06 (2R). RSI(14) ≥50 (bullish bias), MACD cross↑ &amp; above zero with rising histogram; breakout at Donchi</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="n">
+        <v>91.43000000000001</v>
+      </c>
+      <c r="M12" t="n">
+        <v>92.62</v>
+      </c>
+      <c r="N12" t="n">
+        <v>91.09</v>
+      </c>
+      <c r="O12" t="n">
+        <v>93.89</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Pullback Entry: Below EMA20 92.62</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>EMA50-based stop: ₹91.09</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>2R target from entry</t>
+        </is>
+      </c>
+      <c r="S12" t="n">
+        <v>62.26</v>
+      </c>
+      <c r="T12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" t="b">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.1676</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.1767</v>
+      </c>
+      <c r="X12" t="n">
+        <v>-0.0091</v>
+      </c>
+      <c r="Y12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>RSI/MACD fail</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="AG12" t="n">
+        <v/>
+      </c>
+      <c r="AH12" t="n">
+        <v/>
+      </c>
+      <c r="AI12" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="AJ12" t="n">
+        <v>93.89</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>93.89</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>93.90000000000001</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>90.7</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>100.3</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +2216,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1346,13 +2286,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RELIANCE</t>
+          <t>SETFNIFBK</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="7" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -1370,13 +2310,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>INFY</t>
+          <t>SBILIQETF</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C4" s="7" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -1394,13 +2334,13 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NIFTYBEES</t>
+          <t>MOM30IETF</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C5" s="7" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -1418,13 +2358,13 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SETFNIF50</t>
+          <t>FINIETF</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -1438,6 +2378,150 @@
         <v>0</v>
       </c>
       <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>NIFTYETF</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ITETF</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>BSLSENETFG</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>LIQUIDBETF</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BANKBEES</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>PSUBNKBEES</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>